<commit_message>
Login Page and Query Table Test Cases.
</commit_message>
<xml_diff>
--- a/Login_Test_Cases.xlsx
+++ b/Login_Test_Cases.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25524"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{206D7EB7-31E9-4979-9CCC-0D1520BC01F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC48CAF7-7EFB-4CAD-A109-E7506F6BF61A}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>Nbr</t>
   </si>
@@ -68,6 +68,12 @@
     <t>1. UI should be perfect.                  2. Text boxes and buttons should be aligned.</t>
   </si>
   <si>
+    <t>As Expected</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>TC-02</t>
   </si>
   <si>
@@ -83,6 +89,12 @@
     <t>User should not log in and should show proper error message.</t>
   </si>
   <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>TC-03</t>
   </si>
   <si>
@@ -95,6 +107,9 @@
     <t xml:space="preserve">1. Enter vaild username                 2. Enter incorrect password  3. Click on login button </t>
   </si>
   <si>
+    <t xml:space="preserve">Pass </t>
+  </si>
+  <si>
     <t>TC-04</t>
   </si>
   <si>
@@ -158,6 +173,9 @@
     <t>User should get an error message.</t>
   </si>
   <si>
+    <t>Fogot password link is missing.</t>
+  </si>
+  <si>
     <t>TC-09</t>
   </si>
   <si>
@@ -168,6 +186,9 @@
   </si>
   <si>
     <t>1. Go to the reset password link.         2. Enter the previous password. 3. Click on the Reset Password button.</t>
+  </si>
+  <si>
+    <t>Missing</t>
   </si>
   <si>
     <t>TC-10</t>
@@ -219,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +261,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -268,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -281,6 +308,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,25 +685,37 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="76.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="76.5">
@@ -683,19 +723,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="91.5">
@@ -703,19 +749,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="91.5">
@@ -723,19 +775,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="91.5">
@@ -743,19 +801,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45.75">
@@ -763,19 +827,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="106.5">
@@ -783,19 +853,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="106.5">
@@ -803,19 +879,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="121.5">
@@ -823,19 +905,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="137.25">
@@ -843,19 +931,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>42</v>
+      <c r="H12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="152.25">
@@ -863,19 +957,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="121.5">
@@ -883,19 +983,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>